<commit_message>
added color scheme for plotting
</commit_message>
<xml_diff>
--- a/log_data.xlsx
+++ b/log_data.xlsx
@@ -76,16 +76,16 @@
     <t>MIEu</t>
   </si>
   <si>
-    <t>Burgers</t>
-  </si>
-  <si>
-    <t>NetA</t>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>ResNet</t>
   </si>
   <si>
     <t>MSE</t>
   </si>
   <si>
-    <t>2000N63</t>
+    <t>500N63</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
         <v>22</v>
       </c>
       <c r="E2" s="2">
-        <v>44020.78845899536</v>
+        <v>44020.85004700843</v>
       </c>
       <c r="F2" t="s">
         <v>23</v>
@@ -541,7 +541,7 @@
         <v>64</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <v>5</v>
@@ -550,34 +550,34 @@
         <v>32</v>
       </c>
       <c r="L2">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="M2">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="O2">
-        <v>32.816352</v>
+        <v>0.055002</v>
       </c>
       <c r="P2">
-        <v>0.006591</v>
+        <v>0.000267</v>
       </c>
       <c r="Q2">
-        <v>0.731052</v>
+        <v>0.013362</v>
       </c>
       <c r="R2">
-        <v>0.301021</v>
+        <v>0.006681</v>
       </c>
       <c r="S2">
-        <v>0.010622</v>
+        <v>0.000329</v>
       </c>
       <c r="T2">
-        <v>0.210731</v>
+        <v>0.00319</v>
       </c>
       <c r="U2">
-        <v>0.283926</v>
+        <v>0.004525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
push plotting relative_l_inf to l_inf
</commit_message>
<xml_diff>
--- a/log_data.xlsx
+++ b/log_data.xlsx
@@ -79,16 +79,16 @@
     <t>NBFUNCS</t>
   </si>
   <si>
-    <t>Helmholtz</t>
-  </si>
-  <si>
-    <t>ResNet</t>
+    <t>Burgers</t>
+  </si>
+  <si>
+    <t>NetA</t>
   </si>
   <si>
     <t>MSE</t>
   </si>
   <si>
-    <t>100N31</t>
+    <t>1000N31</t>
   </si>
 </sst>
 </file>
@@ -535,7 +535,7 @@
         <v>23</v>
       </c>
       <c r="E2" s="2">
-        <v>44050.87855481443</v>
+        <v>44051.19191161724</v>
       </c>
       <c r="F2" t="s">
         <v>24</v>
@@ -547,7 +547,7 @@
         <v>32</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J2">
         <v>5</v>
@@ -556,37 +556,37 @@
         <v>32</v>
       </c>
       <c r="L2">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="M2">
-        <v>20</v>
+        <v>100000</v>
       </c>
       <c r="N2">
-        <v>1.6</v>
+        <v>0.3</v>
       </c>
       <c r="O2">
-        <v>4448.3175</v>
+        <v>2.304236</v>
       </c>
       <c r="P2">
-        <v>0.181478</v>
+        <v>0.0008630000000000001</v>
       </c>
       <c r="Q2">
-        <v>5.927605</v>
+        <v>0.050889</v>
       </c>
       <c r="R2">
-        <v>3.211066</v>
+        <v>0.045676</v>
       </c>
       <c r="S2">
-        <v>0.227315</v>
+        <v>0.004426</v>
       </c>
       <c r="T2">
-        <v>2.085727</v>
+        <v>0.044978</v>
       </c>
       <c r="U2">
-        <v>3.35058</v>
+        <v>0.045374</v>
       </c>
       <c r="V2">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>